<commit_message>
Add Fouling Data sheet
</commit_message>
<xml_diff>
--- a/Shiny-GAC/Examples/Example_fitter.xlsx
+++ b/Shiny-GAC/Examples/Example_fitter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/burkhardt_jonathan_epa_gov/Documents/Profile/Desktop/Git/GAC_Shiny/4-25-24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/sandlin_cole_epa_gov/Documents/Profile/Documents/GitHub/Water_Treatment_Models/Shiny-GAC/Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{FC6C552E-3166-4C64-8BC2-E954C229B3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4736B8EF-C648-4CEB-B03C-DE0BF2C0E63E}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="8_{FC6C552E-3166-4C64-8BC2-E954C229B3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E6141F7-A768-4A61-A3A3-E25940594120}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2205" windowWidth="51840" windowHeight="21120" activeTab="3" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="columnSpecs" sheetId="4" r:id="rId3"/>
     <sheet name="Notes" sheetId="6" r:id="rId4"/>
     <sheet name="data" sheetId="8" r:id="rId5"/>
+    <sheet name="Fouling Data" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="54">
   <si>
     <t>MW</t>
   </si>
@@ -185,6 +186,18 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>WaterFouling</t>
+  </si>
+  <si>
+    <t>ChemicalFouling</t>
+  </si>
+  <si>
+    <t>Rhine</t>
+  </si>
+  <si>
+    <t>halogenated alkanes</t>
   </si>
 </sst>
 </file>
@@ -272,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -297,6 +310,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,18 +634,18 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -637,7 +653,7 @@
         <v>131.38999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -645,7 +661,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -653,7 +669,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -661,7 +677,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -669,7 +685,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -690,14 +706,14 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -705,7 +721,7 @@
         <v>5026.04</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -713,7 +729,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -721,7 +737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -729,7 +745,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -750,12 +766,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -766,7 +782,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -774,7 +790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -785,7 +801,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -793,7 +809,7 @@
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -801,7 +817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -812,7 +828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
@@ -823,7 +839,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -834,7 +850,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -845,7 +861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -856,7 +872,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -867,7 +883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -875,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -883,7 +899,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -891,7 +907,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -899,7 +915,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
@@ -916,47 +932,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9257DF-418B-48B7-8133-ABF04E7715B5}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="31" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.1796875" style="8"/>
     <col min="2" max="2" width="148" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="63" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.7">
       <c r="B1" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="2:2" ht="63" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:2" ht="62" x14ac:dyDescent="0.7">
       <c r="B2" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="63" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:2" ht="62" x14ac:dyDescent="0.7">
       <c r="B3" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="157.5" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:2" ht="155" x14ac:dyDescent="0.7">
       <c r="B4" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="94.5" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:2" ht="62" x14ac:dyDescent="0.7">
       <c r="B6" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="63" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:2" ht="62" x14ac:dyDescent="0.7">
       <c r="B7" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="63" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:2" ht="62" x14ac:dyDescent="0.7">
       <c r="B9" s="9" t="s">
         <v>47</v>
       </c>
@@ -974,15 +990,15 @@
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -996,7 +1012,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1010,7 +1026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1024,7 +1040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1038,7 +1054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1052,7 +1068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1066,7 +1082,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1080,7 +1096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1094,7 +1110,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1108,7 +1124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1122,7 +1138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1136,7 +1152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1150,7 +1166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1164,7 +1180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1178,7 +1194,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1192,7 +1208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1206,7 +1222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1220,7 +1236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1234,7 +1250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1248,7 +1264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1262,7 +1278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1276,7 +1292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1290,7 +1306,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1304,7 +1320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1318,7 +1334,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1332,7 +1348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1346,7 +1362,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1360,7 +1376,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1372,6 +1388,37 @@
       </c>
       <c r="D28" t="s">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03C3ACB-1853-41AF-AA3F-8E7BBB8C88D9}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1837,6 +1884,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
@@ -1877,20 +1938,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D265CA-67CD-4AD3-99A3-30810910E78A}">
   <ds:schemaRefs>
@@ -1915,6 +1962,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB79E98-5AD2-42D4-8617-624CBCC2A96C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E301F64B-2E68-42FE-B72F-07064BA5C6EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D2AB43-1478-4761-B6C2-35F0AE76DC6E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -1933,20 +1996,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E301F64B-2E68-42FE-B72F-07064BA5C6EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB79E98-5AD2-42D4-8617-624CBCC2A96C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>